<commit_message>
Codes for economic analysis
</commit_message>
<xml_diff>
--- a/misc/mapping.xlsx
+++ b/misc/mapping.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arogy\projects\kathmandu-portal-data\misc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\arogya\projects\c2m2\kathmandu-survey\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="23070" windowHeight="9878"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="18735" windowHeight="9608"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1191" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1426" uniqueCount="523">
   <si>
     <t>variable</t>
   </si>
@@ -1179,6 +1179,417 @@
   </si>
   <si>
     <t>choice_code</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>1 to 3 months</t>
+  </si>
+  <si>
+    <t>4 to 6 months</t>
+  </si>
+  <si>
+    <t>7 to 9 months</t>
+  </si>
+  <si>
+    <t>10 to 11 months</t>
+  </si>
+  <si>
+    <t>25% of last year</t>
+  </si>
+  <si>
+    <t>50% of last year</t>
+  </si>
+  <si>
+    <t>75% of last year</t>
+  </si>
+  <si>
+    <t>Same as last year</t>
+  </si>
+  <si>
+    <t>Income grew</t>
+  </si>
+  <si>
+    <t>Income was almost zero</t>
+  </si>
+  <si>
+    <t>Yes, partially engaged</t>
+  </si>
+  <si>
+    <t>Yes, fully engaged</t>
+  </si>
+  <si>
+    <t>No, completely left</t>
+  </si>
+  <si>
+    <t>No, currently unemployed but looking for work</t>
+  </si>
+  <si>
+    <t>Before March 2020</t>
+  </si>
+  <si>
+    <t>Between March and September 2020</t>
+  </si>
+  <si>
+    <t>Between October and December 2020</t>
+  </si>
+  <si>
+    <t>After December 2021</t>
+  </si>
+  <si>
+    <t>Rotational employment</t>
+  </si>
+  <si>
+    <t>No effect</t>
+  </si>
+  <si>
+    <t>No change due to Covid 19</t>
+  </si>
+  <si>
+    <t>Yes, but I've moved back since</t>
+  </si>
+  <si>
+    <t>Yes, switched to a different neighbourhood</t>
+  </si>
+  <si>
+    <t>Yes, swiched to a new village/city</t>
+  </si>
+  <si>
+    <t>Less than a month</t>
+  </si>
+  <si>
+    <t>2 to 6 months</t>
+  </si>
+  <si>
+    <t>More than 6 months</t>
+  </si>
+  <si>
+    <t>Less than 20 years</t>
+  </si>
+  <si>
+    <t>21 - 40 years</t>
+  </si>
+  <si>
+    <t>41 - 60 years</t>
+  </si>
+  <si>
+    <t>61 and above</t>
+  </si>
+  <si>
+    <t>No education</t>
+  </si>
+  <si>
+    <t>Can read and write</t>
+  </si>
+  <si>
+    <t>SLC or equivalent</t>
+  </si>
+  <si>
+    <t>10+2 or equivalent</t>
+  </si>
+  <si>
+    <t>Undergaduate or equivalent</t>
+  </si>
+  <si>
+    <t>Master's or higher</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Third gender</t>
+  </si>
+  <si>
+    <t>Suryabinayak Municipality</t>
+  </si>
+  <si>
+    <t>Shankharapur Municipality</t>
+  </si>
+  <si>
+    <t>Mahankal Municipality</t>
+  </si>
+  <si>
+    <t>6 to 10 years</t>
+  </si>
+  <si>
+    <t>11 to 15 years</t>
+  </si>
+  <si>
+    <t>15 years or more</t>
+  </si>
+  <si>
+    <t>3 to 5 years</t>
+  </si>
+  <si>
+    <t>0 to 2 years</t>
+  </si>
+  <si>
+    <t>Will reduce by 25%</t>
+  </si>
+  <si>
+    <t>Will stay the same</t>
+  </si>
+  <si>
+    <t>Will reduce by 50%</t>
+  </si>
+  <si>
+    <t>Will reduce by 75%</t>
+  </si>
+  <si>
+    <t>Will reduce to zero</t>
+  </si>
+  <si>
+    <t>Will grow</t>
+  </si>
+  <si>
+    <t>Less than 6 months</t>
+  </si>
+  <si>
+    <t>6 to 12 months</t>
+  </si>
+  <si>
+    <t>13 to 24 months</t>
+  </si>
+  <si>
+    <t>24 months or more</t>
+  </si>
+  <si>
+    <t>Immediately</t>
+  </si>
+  <si>
+    <t>Within 3 months</t>
+  </si>
+  <si>
+    <t>Within 12 months</t>
+  </si>
+  <si>
+    <t>Can't say</t>
+  </si>
+  <si>
+    <t>I'm planning to leave the tourism sector</t>
+  </si>
+  <si>
+    <t>Has stayed the same</t>
+  </si>
+  <si>
+    <t>Has reduced to 75%</t>
+  </si>
+  <si>
+    <t>Has reduced to 50%</t>
+  </si>
+  <si>
+    <t>Has reduced to 25%</t>
+  </si>
+  <si>
+    <t>Has reduced to zero</t>
+  </si>
+  <si>
+    <t>Has grown</t>
+  </si>
+  <si>
+    <t>Only me</t>
+  </si>
+  <si>
+    <t>2 people</t>
+  </si>
+  <si>
+    <t>3 to 5 people</t>
+  </si>
+  <si>
+    <t>6 people or more</t>
+  </si>
+  <si>
+    <t>Family and friends</t>
+  </si>
+  <si>
+    <t>Social media</t>
+  </si>
+  <si>
+    <t>Radio</t>
+  </si>
+  <si>
+    <t>Television</t>
+  </si>
+  <si>
+    <t>Newspapers</t>
+  </si>
+  <si>
+    <t>Nearby health service provider</t>
+  </si>
+  <si>
+    <t>Government</t>
+  </si>
+  <si>
+    <t>NGO</t>
+  </si>
+  <si>
+    <t>Employer</t>
+  </si>
+  <si>
+    <t>Hotel / workers associations</t>
+  </si>
+  <si>
+    <t>Land</t>
+  </si>
+  <si>
+    <t>Cable TV connection</t>
+  </si>
+  <si>
+    <t>Computer / laptop</t>
+  </si>
+  <si>
+    <t>Internet</t>
+  </si>
+  <si>
+    <t>Telephone</t>
+  </si>
+  <si>
+    <t>Mobile phone</t>
+  </si>
+  <si>
+    <t>Refrigerator</t>
+  </si>
+  <si>
+    <t>Motorcycle</t>
+  </si>
+  <si>
+    <t>Four wheeler for self/family use</t>
+  </si>
+  <si>
+    <t>Four wheeler for commercial use</t>
+  </si>
+  <si>
+    <t>None of the above</t>
+  </si>
+  <si>
+    <t>Seasonal work</t>
+  </si>
+  <si>
+    <t>Daily wages</t>
+  </si>
+  <si>
+    <t>Monthly salary</t>
+  </si>
+  <si>
+    <t>Shopkeeper</t>
+  </si>
+  <si>
+    <t>Tour guide</t>
+  </si>
+  <si>
+    <t>Trekking guide</t>
+  </si>
+  <si>
+    <t>Rafting guide</t>
+  </si>
+  <si>
+    <t>Mountain guide</t>
+  </si>
+  <si>
+    <t>Driver</t>
+  </si>
+  <si>
+    <t>Travel agent</t>
+  </si>
+  <si>
+    <t>Flight attendant</t>
+  </si>
+  <si>
+    <t>Pilot</t>
+  </si>
+  <si>
+    <t>Chef / cook</t>
+  </si>
+  <si>
+    <t>Hotel manager</t>
+  </si>
+  <si>
+    <t>Hotel staff</t>
+  </si>
+  <si>
+    <t>Waiter</t>
+  </si>
+  <si>
+    <t>Bartender</t>
+  </si>
+  <si>
+    <t>Porter</t>
+  </si>
+  <si>
+    <t>Loan through financial institutions</t>
+  </si>
+  <si>
+    <t>Loan through friends and family</t>
+  </si>
+  <si>
+    <t>Stopped education of a family member</t>
+  </si>
+  <si>
+    <t>Stopped health services for family members</t>
+  </si>
+  <si>
+    <t>Sold personal assets</t>
+  </si>
+  <si>
+    <t>Sold professional assets (camera, etc.)</t>
+  </si>
+  <si>
+    <t>Sold land or property</t>
+  </si>
+  <si>
+    <t>Lost job</t>
+  </si>
+  <si>
+    <t>Lost self-employment</t>
+  </si>
+  <si>
+    <t>Salary cut</t>
+  </si>
+  <si>
+    <t>Couldn't renew licences and permits</t>
+  </si>
+  <si>
+    <t>Took up ininteresting job</t>
+  </si>
+  <si>
+    <t>Winning tourists confidence</t>
+  </si>
+  <si>
+    <t>Ensuring HHS Compliance\</t>
+  </si>
+  <si>
+    <t>Overcoming financial challenges</t>
+  </si>
+  <si>
+    <t>Difficulty paying for health services</t>
+  </si>
+  <si>
+    <t>Difficulty paying for education</t>
+  </si>
+  <si>
+    <t>Difficulty paying for food</t>
+  </si>
+  <si>
+    <t>o_impct_to_self_nxt_6_mnths_rnk_1</t>
+  </si>
+  <si>
+    <t>Difficulty covering rent</t>
+  </si>
+  <si>
+    <t>Difficulty covering rent (partial amount)</t>
+  </si>
+  <si>
+    <t>Difficulty in borrowing cash</t>
+  </si>
+  <si>
+    <t>Difficulty in repaying existing debt</t>
   </si>
 </sst>
 </file>
@@ -1458,15 +1869,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F476"/>
+  <dimension ref="A1:F485"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A460" workbookViewId="0">
-      <selection activeCell="E476" sqref="E476"/>
+    <sheetView tabSelected="1" topLeftCell="A469" workbookViewId="0">
+      <selection activeCell="D483" sqref="D483"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.73046875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.73046875" customWidth="1"/>
   </cols>
@@ -1501,7 +1912,9 @@
       <c r="C2" s="2">
         <v>1</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>386</v>
+      </c>
       <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1519,7 +1932,9 @@
       <c r="C3" s="2">
         <v>2</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>387</v>
+      </c>
       <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
@@ -1537,7 +1952,9 @@
       <c r="C4" s="2">
         <v>3</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>386</v>
+      </c>
       <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1555,7 +1972,9 @@
       <c r="C5" s="2">
         <v>4</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="1" t="s">
+        <v>387</v>
+      </c>
       <c r="E5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1573,7 +1992,9 @@
       <c r="C6" s="2">
         <v>5</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>388</v>
+      </c>
       <c r="E6" s="1" t="s">
         <v>12</v>
       </c>
@@ -1589,7 +2010,9 @@
       <c r="C7" s="2">
         <v>6</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>389</v>
+      </c>
       <c r="E7" s="1" t="s">
         <v>13</v>
       </c>
@@ -1605,7 +2028,9 @@
       <c r="C8" s="2">
         <v>7</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>390</v>
+      </c>
       <c r="E8" s="1" t="s">
         <v>14</v>
       </c>
@@ -1621,7 +2046,9 @@
       <c r="C9" s="2">
         <v>8</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>391</v>
+      </c>
       <c r="E9" s="1" t="s">
         <v>15</v>
       </c>
@@ -1637,7 +2064,9 @@
       <c r="C10" s="2">
         <v>9</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>397</v>
+      </c>
       <c r="E10" s="1" t="s">
         <v>17</v>
       </c>
@@ -1653,7 +2082,9 @@
       <c r="C11" s="2">
         <v>10</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>392</v>
+      </c>
       <c r="E11" s="1" t="s">
         <v>18</v>
       </c>
@@ -1669,7 +2100,9 @@
       <c r="C12" s="2">
         <v>11</v>
       </c>
-      <c r="D12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>393</v>
+      </c>
       <c r="E12" s="1" t="s">
         <v>19</v>
       </c>
@@ -1685,7 +2118,9 @@
       <c r="C13" s="2">
         <v>12</v>
       </c>
-      <c r="D13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>394</v>
+      </c>
       <c r="E13" s="1" t="s">
         <v>20</v>
       </c>
@@ -1701,7 +2136,9 @@
       <c r="C14" s="2">
         <v>13</v>
       </c>
-      <c r="D14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>395</v>
+      </c>
       <c r="E14" s="1" t="s">
         <v>21</v>
       </c>
@@ -1717,7 +2154,9 @@
       <c r="C15" s="2">
         <v>14</v>
       </c>
-      <c r="D15" s="1"/>
+      <c r="D15" s="1" t="s">
+        <v>396</v>
+      </c>
       <c r="E15" s="1" t="s">
         <v>22</v>
       </c>
@@ -1733,7 +2172,9 @@
       <c r="C16" s="2">
         <v>15</v>
       </c>
-      <c r="D16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>386</v>
+      </c>
       <c r="E16" s="1" t="s">
         <v>24</v>
       </c>
@@ -1749,7 +2190,9 @@
       <c r="C17" s="2">
         <v>16</v>
       </c>
-      <c r="D17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>387</v>
+      </c>
       <c r="E17" s="1" t="s">
         <v>25</v>
       </c>
@@ -1765,7 +2208,9 @@
       <c r="C18" s="2">
         <v>17</v>
       </c>
-      <c r="D18" s="1"/>
+      <c r="D18" s="1" t="s">
+        <v>386</v>
+      </c>
       <c r="E18" s="1" t="s">
         <v>24</v>
       </c>
@@ -1781,7 +2226,9 @@
       <c r="C19" s="2">
         <v>18</v>
       </c>
-      <c r="D19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>387</v>
+      </c>
       <c r="E19" s="1" t="s">
         <v>25</v>
       </c>
@@ -1797,7 +2244,9 @@
       <c r="C20" s="2">
         <v>19</v>
       </c>
-      <c r="D20" s="1"/>
+      <c r="D20" s="1" t="s">
+        <v>386</v>
+      </c>
       <c r="E20" s="1" t="s">
         <v>28</v>
       </c>
@@ -1813,7 +2262,9 @@
       <c r="C21" s="2">
         <v>20</v>
       </c>
-      <c r="D21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>387</v>
+      </c>
       <c r="E21" s="1" t="s">
         <v>29</v>
       </c>
@@ -1829,7 +2280,9 @@
       <c r="C22" s="2">
         <v>21</v>
       </c>
-      <c r="D22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>386</v>
+      </c>
       <c r="E22" s="1" t="s">
         <v>31</v>
       </c>
@@ -1845,7 +2298,9 @@
       <c r="C23" s="2">
         <v>22</v>
       </c>
-      <c r="D23" s="1"/>
+      <c r="D23" s="1" t="s">
+        <v>387</v>
+      </c>
       <c r="E23" s="1" t="s">
         <v>32</v>
       </c>
@@ -1861,7 +2316,9 @@
       <c r="C24" s="2">
         <v>23</v>
       </c>
-      <c r="D24" s="1"/>
+      <c r="D24" s="1" t="s">
+        <v>399</v>
+      </c>
       <c r="E24" s="1" t="s">
         <v>34</v>
       </c>
@@ -1877,7 +2334,9 @@
       <c r="C25" s="2">
         <v>24</v>
       </c>
-      <c r="D25" s="1"/>
+      <c r="D25" s="1" t="s">
+        <v>398</v>
+      </c>
       <c r="E25" s="1" t="s">
         <v>35</v>
       </c>
@@ -1893,7 +2352,9 @@
       <c r="C26" s="2">
         <v>25</v>
       </c>
-      <c r="D26" s="1"/>
+      <c r="D26" s="1" t="s">
+        <v>401</v>
+      </c>
       <c r="E26" s="1" t="s">
         <v>36</v>
       </c>
@@ -1909,7 +2370,9 @@
       <c r="C27" s="2">
         <v>26</v>
       </c>
-      <c r="D27" s="1"/>
+      <c r="D27" s="1" t="s">
+        <v>400</v>
+      </c>
       <c r="E27" s="1" t="s">
         <v>37</v>
       </c>
@@ -1925,7 +2388,9 @@
       <c r="C28" s="2">
         <v>27</v>
       </c>
-      <c r="D28" s="1"/>
+      <c r="D28" s="1" t="s">
+        <v>402</v>
+      </c>
       <c r="E28" s="1" t="s">
         <v>39</v>
       </c>
@@ -1941,7 +2406,9 @@
       <c r="C29" s="2">
         <v>28</v>
       </c>
-      <c r="D29" s="1"/>
+      <c r="D29" s="1" t="s">
+        <v>403</v>
+      </c>
       <c r="E29" s="1" t="s">
         <v>40</v>
       </c>
@@ -1957,7 +2424,9 @@
       <c r="C30" s="2">
         <v>29</v>
       </c>
-      <c r="D30" s="1"/>
+      <c r="D30" s="1" t="s">
+        <v>404</v>
+      </c>
       <c r="E30" s="1" t="s">
         <v>41</v>
       </c>
@@ -1973,7 +2442,9 @@
       <c r="C31" s="2">
         <v>30</v>
       </c>
-      <c r="D31" s="1"/>
+      <c r="D31" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="E31" s="1" t="s">
         <v>42</v>
       </c>
@@ -1989,7 +2460,9 @@
       <c r="C32" s="2">
         <v>31</v>
       </c>
-      <c r="D32" s="1"/>
+      <c r="D32" s="1" t="s">
+        <v>408</v>
+      </c>
       <c r="E32" s="1" t="s">
         <v>43</v>
       </c>
@@ -2005,7 +2478,9 @@
       <c r="C33" s="2">
         <v>32</v>
       </c>
-      <c r="D33" s="1"/>
+      <c r="D33" s="1" t="s">
+        <v>386</v>
+      </c>
       <c r="E33" s="1" t="s">
         <v>6</v>
       </c>
@@ -2021,7 +2496,9 @@
       <c r="C34" s="2">
         <v>33</v>
       </c>
-      <c r="D34" s="1"/>
+      <c r="D34" s="1" t="s">
+        <v>387</v>
+      </c>
       <c r="E34" s="1" t="s">
         <v>7</v>
       </c>
@@ -2037,7 +2514,9 @@
       <c r="C35" s="2">
         <v>34</v>
       </c>
-      <c r="D35" s="1"/>
+      <c r="D35" s="1" t="s">
+        <v>386</v>
+      </c>
       <c r="E35" s="1" t="s">
         <v>6</v>
       </c>
@@ -2053,7 +2532,9 @@
       <c r="C36" s="2">
         <v>35</v>
       </c>
-      <c r="D36" s="1"/>
+      <c r="D36" s="1" t="s">
+        <v>387</v>
+      </c>
       <c r="E36" s="1" t="s">
         <v>7</v>
       </c>
@@ -2069,7 +2550,9 @@
       <c r="C37" s="2">
         <v>36</v>
       </c>
-      <c r="D37" s="1"/>
+      <c r="D37" s="1" t="s">
+        <v>403</v>
+      </c>
       <c r="E37" s="1" t="s">
         <v>40</v>
       </c>
@@ -2085,7 +2568,9 @@
       <c r="C38" s="2">
         <v>37</v>
       </c>
-      <c r="D38" s="1"/>
+      <c r="D38" s="1" t="s">
+        <v>404</v>
+      </c>
       <c r="E38" s="1" t="s">
         <v>41</v>
       </c>
@@ -2101,7 +2586,9 @@
       <c r="C39" s="2">
         <v>38</v>
       </c>
-      <c r="D39" s="1"/>
+      <c r="D39" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="E39" s="1" t="s">
         <v>42</v>
       </c>
@@ -2117,7 +2604,9 @@
       <c r="C40" s="2">
         <v>39</v>
       </c>
-      <c r="D40" s="1"/>
+      <c r="D40" s="1" t="s">
+        <v>409</v>
+      </c>
       <c r="E40" s="1" t="s">
         <v>48</v>
       </c>
@@ -2133,7 +2622,9 @@
       <c r="C41" s="2">
         <v>40</v>
       </c>
-      <c r="D41" s="1"/>
+      <c r="D41" s="1" t="s">
+        <v>410</v>
+      </c>
       <c r="E41" s="1" t="s">
         <v>49</v>
       </c>
@@ -2149,7 +2640,9 @@
       <c r="C42" s="2">
         <v>41</v>
       </c>
-      <c r="D42" s="1"/>
+      <c r="D42" s="1" t="s">
+        <v>411</v>
+      </c>
       <c r="E42" s="1" t="s">
         <v>50</v>
       </c>
@@ -2165,7 +2658,9 @@
       <c r="C43" s="2">
         <v>42</v>
       </c>
-      <c r="D43" s="1"/>
+      <c r="D43" s="1" t="s">
+        <v>387</v>
+      </c>
       <c r="E43" s="1" t="s">
         <v>25</v>
       </c>
@@ -2181,7 +2676,9 @@
       <c r="C44" s="2">
         <v>43</v>
       </c>
-      <c r="D44" s="1"/>
+      <c r="D44" s="1" t="s">
+        <v>412</v>
+      </c>
       <c r="E44" s="1" t="s">
         <v>52</v>
       </c>
@@ -2197,7 +2694,9 @@
       <c r="C45" s="2">
         <v>44</v>
       </c>
-      <c r="D45" s="1"/>
+      <c r="D45" s="1" t="s">
+        <v>413</v>
+      </c>
       <c r="E45" s="1" t="s">
         <v>53</v>
       </c>
@@ -2213,7 +2712,9 @@
       <c r="C46" s="2">
         <v>45</v>
       </c>
-      <c r="D46" s="1"/>
+      <c r="D46" s="1" t="s">
+        <v>414</v>
+      </c>
       <c r="E46" s="1" t="s">
         <v>54</v>
       </c>
@@ -2229,7 +2730,9 @@
       <c r="C47" s="2">
         <v>46</v>
       </c>
-      <c r="D47" s="1"/>
+      <c r="D47" s="1" t="s">
+        <v>387</v>
+      </c>
       <c r="E47" s="1" t="s">
         <v>29</v>
       </c>
@@ -2245,7 +2748,9 @@
       <c r="C48" s="2">
         <v>47</v>
       </c>
-      <c r="D48" s="1"/>
+      <c r="D48" s="1" t="s">
+        <v>386</v>
+      </c>
       <c r="E48" s="1" t="s">
         <v>28</v>
       </c>
@@ -2261,7 +2766,9 @@
       <c r="C49" s="2">
         <v>48</v>
       </c>
-      <c r="D49" s="1"/>
+      <c r="D49" s="1" t="s">
+        <v>387</v>
+      </c>
       <c r="E49" s="1" t="s">
         <v>29</v>
       </c>
@@ -2277,7 +2784,9 @@
       <c r="C50" s="2">
         <v>49</v>
       </c>
-      <c r="D50" s="1"/>
+      <c r="D50" s="1" t="s">
+        <v>386</v>
+      </c>
       <c r="E50" s="1" t="s">
         <v>28</v>
       </c>
@@ -2293,7 +2802,9 @@
       <c r="C51" s="2">
         <v>50</v>
       </c>
-      <c r="D51" s="1"/>
+      <c r="D51" s="1" t="s">
+        <v>387</v>
+      </c>
       <c r="E51" s="1" t="s">
         <v>29</v>
       </c>
@@ -2309,7 +2820,9 @@
       <c r="C52" s="2">
         <v>51</v>
       </c>
-      <c r="D52" s="1"/>
+      <c r="D52" s="1" t="s">
+        <v>386</v>
+      </c>
       <c r="E52" s="1" t="s">
         <v>28</v>
       </c>
@@ -2325,7 +2838,9 @@
       <c r="C53" s="2">
         <v>52</v>
       </c>
-      <c r="D53" s="1"/>
+      <c r="D53" s="1" t="s">
+        <v>387</v>
+      </c>
       <c r="E53" s="1" t="s">
         <v>29</v>
       </c>
@@ -2341,7 +2856,9 @@
       <c r="C54" s="2">
         <v>53</v>
       </c>
-      <c r="D54" s="1"/>
+      <c r="D54" s="1" t="s">
+        <v>386</v>
+      </c>
       <c r="E54" s="1" t="s">
         <v>28</v>
       </c>
@@ -2357,7 +2874,9 @@
       <c r="C55" s="2">
         <v>54</v>
       </c>
-      <c r="D55" s="1"/>
+      <c r="D55" s="1" t="s">
+        <v>387</v>
+      </c>
       <c r="E55" s="1" t="s">
         <v>29</v>
       </c>
@@ -2373,7 +2892,9 @@
       <c r="C56" s="2">
         <v>55</v>
       </c>
-      <c r="D56" s="1"/>
+      <c r="D56" s="1" t="s">
+        <v>386</v>
+      </c>
       <c r="E56" s="1" t="s">
         <v>28</v>
       </c>
@@ -2389,7 +2910,9 @@
       <c r="C57" s="2">
         <v>56</v>
       </c>
-      <c r="D57" s="1"/>
+      <c r="D57" s="1" t="s">
+        <v>387</v>
+      </c>
       <c r="E57" s="1" t="s">
         <v>29</v>
       </c>
@@ -2405,7 +2928,9 @@
       <c r="C58" s="2">
         <v>57</v>
       </c>
-      <c r="D58" s="1"/>
+      <c r="D58" s="1" t="s">
+        <v>386</v>
+      </c>
       <c r="E58" s="1" t="s">
         <v>28</v>
       </c>
@@ -2421,7 +2946,9 @@
       <c r="C59" s="2">
         <v>58</v>
       </c>
-      <c r="D59" s="1"/>
+      <c r="D59" s="1" t="s">
+        <v>387</v>
+      </c>
       <c r="E59" s="1" t="s">
         <v>29</v>
       </c>
@@ -2437,7 +2964,9 @@
       <c r="C60" s="2">
         <v>59</v>
       </c>
-      <c r="D60" s="1"/>
+      <c r="D60" s="1" t="s">
+        <v>386</v>
+      </c>
       <c r="E60" s="1" t="s">
         <v>28</v>
       </c>
@@ -2453,7 +2982,9 @@
       <c r="C61" s="2">
         <v>60</v>
       </c>
-      <c r="D61" s="1"/>
+      <c r="D61" s="1" t="s">
+        <v>387</v>
+      </c>
       <c r="E61" s="1" t="s">
         <v>29</v>
       </c>
@@ -2469,7 +3000,9 @@
       <c r="C62" s="2">
         <v>61</v>
       </c>
-      <c r="D62" s="1"/>
+      <c r="D62" s="1" t="s">
+        <v>386</v>
+      </c>
       <c r="E62" s="1" t="s">
         <v>28</v>
       </c>
@@ -2485,7 +3018,9 @@
       <c r="C63" s="2">
         <v>62</v>
       </c>
-      <c r="D63" s="1"/>
+      <c r="D63" s="1" t="s">
+        <v>415</v>
+      </c>
       <c r="E63" s="1" t="s">
         <v>64</v>
       </c>
@@ -2501,7 +3036,9 @@
       <c r="C64" s="2">
         <v>63</v>
       </c>
-      <c r="D64" s="1"/>
+      <c r="D64" s="1" t="s">
+        <v>416</v>
+      </c>
       <c r="E64" s="1" t="s">
         <v>65</v>
       </c>
@@ -2517,7 +3054,9 @@
       <c r="C65" s="2">
         <v>64</v>
       </c>
-      <c r="D65" s="1"/>
+      <c r="D65" s="1" t="s">
+        <v>417</v>
+      </c>
       <c r="E65" s="1" t="s">
         <v>66</v>
       </c>
@@ -2533,7 +3072,9 @@
       <c r="C66" s="2">
         <v>65</v>
       </c>
-      <c r="D66" s="1"/>
+      <c r="D66" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="E66" s="1" t="s">
         <v>67</v>
       </c>
@@ -5321,7 +5862,9 @@
       <c r="C221" s="2">
         <v>220</v>
       </c>
-      <c r="D221" s="1"/>
+      <c r="D221" s="1" t="s">
+        <v>419</v>
+      </c>
       <c r="E221" s="1" t="s">
         <v>225</v>
       </c>
@@ -5337,7 +5880,9 @@
       <c r="C222" s="2">
         <v>221</v>
       </c>
-      <c r="D222" s="1"/>
+      <c r="D222" s="1" t="s">
+        <v>420</v>
+      </c>
       <c r="E222" s="1" t="s">
         <v>226</v>
       </c>
@@ -5353,7 +5898,9 @@
       <c r="C223" s="2">
         <v>222</v>
       </c>
-      <c r="D223" s="1"/>
+      <c r="D223" s="1" t="s">
+        <v>421</v>
+      </c>
       <c r="E223" s="1" t="s">
         <v>227</v>
       </c>
@@ -5369,7 +5916,9 @@
       <c r="C224" s="2">
         <v>223</v>
       </c>
-      <c r="D224" s="1"/>
+      <c r="D224" s="1" t="s">
+        <v>422</v>
+      </c>
       <c r="E224" s="3" t="s">
         <v>228</v>
       </c>
@@ -5385,7 +5934,9 @@
       <c r="C225" s="2">
         <v>224</v>
       </c>
-      <c r="D225" s="1"/>
+      <c r="D225" s="1" t="s">
+        <v>423</v>
+      </c>
       <c r="E225" s="1" t="s">
         <v>229</v>
       </c>
@@ -5401,7 +5952,9 @@
       <c r="C226" s="2">
         <v>225</v>
       </c>
-      <c r="D226" s="1"/>
+      <c r="D226" s="1" t="s">
+        <v>424</v>
+      </c>
       <c r="E226" s="1" t="s">
         <v>230</v>
       </c>
@@ -5417,7 +5970,9 @@
       <c r="C227" s="2">
         <v>226</v>
       </c>
-      <c r="D227" s="1"/>
+      <c r="D227" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="E227" s="1" t="s">
         <v>232</v>
       </c>
@@ -5433,7 +5988,9 @@
       <c r="C228" s="2">
         <v>227</v>
       </c>
-      <c r="D228" s="1"/>
+      <c r="D228" s="1" t="s">
+        <v>426</v>
+      </c>
       <c r="E228" s="1" t="s">
         <v>233</v>
       </c>
@@ -5449,7 +6006,9 @@
       <c r="C229" s="2">
         <v>228</v>
       </c>
-      <c r="D229" s="1"/>
+      <c r="D229" s="1" t="s">
+        <v>427</v>
+      </c>
       <c r="E229" s="1" t="s">
         <v>234</v>
       </c>
@@ -5465,7 +6024,9 @@
       <c r="C230" s="2">
         <v>229</v>
       </c>
-      <c r="D230" s="1"/>
+      <c r="D230" s="1" t="s">
+        <v>428</v>
+      </c>
       <c r="E230" s="1" t="s">
         <v>236</v>
       </c>
@@ -5481,7 +6042,9 @@
       <c r="C231" s="2">
         <v>230</v>
       </c>
-      <c r="D231" s="1"/>
+      <c r="D231" s="1" t="s">
+        <v>429</v>
+      </c>
       <c r="E231" s="1" t="s">
         <v>237</v>
       </c>
@@ -5497,7 +6060,9 @@
       <c r="C232" s="2">
         <v>231</v>
       </c>
-      <c r="D232" s="1"/>
+      <c r="D232" s="1" t="s">
+        <v>430</v>
+      </c>
       <c r="E232" s="1" t="s">
         <v>238</v>
       </c>
@@ -5513,7 +6078,9 @@
       <c r="C233" s="2">
         <v>232</v>
       </c>
-      <c r="D233" s="1"/>
+      <c r="D233" s="1" t="s">
+        <v>428</v>
+      </c>
       <c r="E233" s="1" t="s">
         <v>236</v>
       </c>
@@ -5529,7 +6096,9 @@
       <c r="C234" s="2">
         <v>233</v>
       </c>
-      <c r="D234" s="1"/>
+      <c r="D234" s="1" t="s">
+        <v>429</v>
+      </c>
       <c r="E234" s="1" t="s">
         <v>237</v>
       </c>
@@ -5545,7 +6114,9 @@
       <c r="C235" s="2">
         <v>234</v>
       </c>
-      <c r="D235" s="1"/>
+      <c r="D235" s="1" t="s">
+        <v>430</v>
+      </c>
       <c r="E235" s="1" t="s">
         <v>238</v>
       </c>
@@ -5561,7 +6132,9 @@
       <c r="C236" s="2">
         <v>235</v>
       </c>
-      <c r="D236" s="1"/>
+      <c r="D236" s="1" t="s">
+        <v>435</v>
+      </c>
       <c r="E236" s="1" t="s">
         <v>241</v>
       </c>
@@ -5577,7 +6150,9 @@
       <c r="C237" s="2">
         <v>236</v>
       </c>
-      <c r="D237" s="1"/>
+      <c r="D237" s="1" t="s">
+        <v>434</v>
+      </c>
       <c r="E237" s="1" t="s">
         <v>242</v>
       </c>
@@ -5593,7 +6168,9 @@
       <c r="C238" s="2">
         <v>237</v>
       </c>
-      <c r="D238" s="1"/>
+      <c r="D238" s="1" t="s">
+        <v>431</v>
+      </c>
       <c r="E238" s="1" t="s">
         <v>243</v>
       </c>
@@ -5609,7 +6186,9 @@
       <c r="C239" s="2">
         <v>238</v>
       </c>
-      <c r="D239" s="1"/>
+      <c r="D239" s="1" t="s">
+        <v>432</v>
+      </c>
       <c r="E239" s="1" t="s">
         <v>244</v>
       </c>
@@ -5625,7 +6204,9 @@
       <c r="C240" s="2">
         <v>239</v>
       </c>
-      <c r="D240" s="1"/>
+      <c r="D240" s="1" t="s">
+        <v>433</v>
+      </c>
       <c r="E240" s="1" t="s">
         <v>245</v>
       </c>
@@ -5641,7 +6222,9 @@
       <c r="C241" s="2">
         <v>240</v>
       </c>
-      <c r="D241" s="1"/>
+      <c r="D241" s="1" t="s">
+        <v>437</v>
+      </c>
       <c r="E241" s="1" t="s">
         <v>247</v>
       </c>
@@ -5657,7 +6240,9 @@
       <c r="C242" s="2">
         <v>241</v>
       </c>
-      <c r="D242" s="1"/>
+      <c r="D242" s="1" t="s">
+        <v>436</v>
+      </c>
       <c r="E242" s="1" t="s">
         <v>248</v>
       </c>
@@ -5673,7 +6258,9 @@
       <c r="C243" s="2">
         <v>242</v>
       </c>
-      <c r="D243" s="1"/>
+      <c r="D243" s="1" t="s">
+        <v>438</v>
+      </c>
       <c r="E243" s="1" t="s">
         <v>249</v>
       </c>
@@ -5689,7 +6276,9 @@
       <c r="C244" s="2">
         <v>243</v>
       </c>
-      <c r="D244" s="1"/>
+      <c r="D244" s="1" t="s">
+        <v>439</v>
+      </c>
       <c r="E244" s="1" t="s">
         <v>250</v>
       </c>
@@ -5705,7 +6294,9 @@
       <c r="C245" s="2">
         <v>244</v>
       </c>
-      <c r="D245" s="1"/>
+      <c r="D245" s="1" t="s">
+        <v>440</v>
+      </c>
       <c r="E245" s="1" t="s">
         <v>251</v>
       </c>
@@ -5721,7 +6312,9 @@
       <c r="C246" s="2">
         <v>245</v>
       </c>
-      <c r="D246" s="1"/>
+      <c r="D246" s="1" t="s">
+        <v>441</v>
+      </c>
       <c r="E246" s="1" t="s">
         <v>252</v>
       </c>
@@ -5737,7 +6330,9 @@
       <c r="C247" s="2">
         <v>246</v>
       </c>
-      <c r="D247" s="1"/>
+      <c r="D247" s="1" t="s">
+        <v>442</v>
+      </c>
       <c r="E247" s="1" t="s">
         <v>254</v>
       </c>
@@ -5753,7 +6348,9 @@
       <c r="C248" s="2">
         <v>247</v>
       </c>
-      <c r="D248" s="1"/>
+      <c r="D248" s="1" t="s">
+        <v>443</v>
+      </c>
       <c r="E248" s="1" t="s">
         <v>255</v>
       </c>
@@ -5769,7 +6366,9 @@
       <c r="C249" s="2">
         <v>248</v>
       </c>
-      <c r="D249" s="1"/>
+      <c r="D249" s="1" t="s">
+        <v>444</v>
+      </c>
       <c r="E249" s="1" t="s">
         <v>256</v>
       </c>
@@ -5785,7 +6384,9 @@
       <c r="C250" s="2">
         <v>249</v>
       </c>
-      <c r="D250" s="1"/>
+      <c r="D250" s="1" t="s">
+        <v>445</v>
+      </c>
       <c r="E250" s="1" t="s">
         <v>257</v>
       </c>
@@ -5801,7 +6402,9 @@
       <c r="C251" s="2">
         <v>250</v>
       </c>
-      <c r="D251" s="1"/>
+      <c r="D251" s="1" t="s">
+        <v>446</v>
+      </c>
       <c r="E251" s="1" t="s">
         <v>259</v>
       </c>
@@ -5817,7 +6420,9 @@
       <c r="C252" s="2">
         <v>251</v>
       </c>
-      <c r="D252" s="1"/>
+      <c r="D252" s="1" t="s">
+        <v>447</v>
+      </c>
       <c r="E252" s="1" t="s">
         <v>260</v>
       </c>
@@ -5833,7 +6438,9 @@
       <c r="C253" s="2">
         <v>252</v>
       </c>
-      <c r="D253" s="1"/>
+      <c r="D253" s="1" t="s">
+        <v>448</v>
+      </c>
       <c r="E253" s="1" t="s">
         <v>261</v>
       </c>
@@ -5849,7 +6456,9 @@
       <c r="C254" s="2">
         <v>253</v>
       </c>
-      <c r="D254" s="1"/>
+      <c r="D254" s="1" t="s">
+        <v>450</v>
+      </c>
       <c r="E254" s="1" t="s">
         <v>262</v>
       </c>
@@ -5865,7 +6474,9 @@
       <c r="C255" s="2">
         <v>254</v>
       </c>
-      <c r="D255" s="1"/>
+      <c r="D255" s="1" t="s">
+        <v>449</v>
+      </c>
       <c r="E255" s="1" t="s">
         <v>263</v>
       </c>
@@ -5881,7 +6492,9 @@
       <c r="C256" s="2">
         <v>255</v>
       </c>
-      <c r="D256" s="1"/>
+      <c r="D256" s="1" t="s">
+        <v>387</v>
+      </c>
       <c r="E256" s="1" t="s">
         <v>29</v>
       </c>
@@ -5897,7 +6510,9 @@
       <c r="C257" s="2">
         <v>256</v>
       </c>
-      <c r="D257" s="1"/>
+      <c r="D257" s="1" t="s">
+        <v>386</v>
+      </c>
       <c r="E257" s="1" t="s">
         <v>28</v>
       </c>
@@ -5913,7 +6528,9 @@
       <c r="C258" s="2">
         <v>257</v>
       </c>
-      <c r="D258" s="1"/>
+      <c r="D258" s="1" t="s">
+        <v>451</v>
+      </c>
       <c r="E258" s="1" t="s">
         <v>266</v>
       </c>
@@ -5929,7 +6546,9 @@
       <c r="C259" s="2">
         <v>258</v>
       </c>
-      <c r="D259" s="1"/>
+      <c r="D259" s="1" t="s">
+        <v>452</v>
+      </c>
       <c r="E259" s="1" t="s">
         <v>267</v>
       </c>
@@ -5945,7 +6564,9 @@
       <c r="C260" s="2">
         <v>259</v>
       </c>
-      <c r="D260" s="1"/>
+      <c r="D260" s="1" t="s">
+        <v>453</v>
+      </c>
       <c r="E260" s="1" t="s">
         <v>268</v>
       </c>
@@ -5961,7 +6582,9 @@
       <c r="C261" s="2">
         <v>260</v>
       </c>
-      <c r="D261" s="1"/>
+      <c r="D261" s="1" t="s">
+        <v>454</v>
+      </c>
       <c r="E261" s="1" t="s">
         <v>269</v>
       </c>
@@ -5977,7 +6600,9 @@
       <c r="C262" s="2">
         <v>261</v>
       </c>
-      <c r="D262" s="1"/>
+      <c r="D262" s="1" t="s">
+        <v>455</v>
+      </c>
       <c r="E262" s="1" t="s">
         <v>270</v>
       </c>
@@ -5993,7 +6618,9 @@
       <c r="C263" s="2">
         <v>262</v>
       </c>
-      <c r="D263" s="1"/>
+      <c r="D263" s="1" t="s">
+        <v>456</v>
+      </c>
       <c r="E263" s="1" t="s">
         <v>271</v>
       </c>
@@ -6009,7 +6636,9 @@
       <c r="C264" s="2">
         <v>263</v>
       </c>
-      <c r="D264" s="1"/>
+      <c r="D264" s="1" t="s">
+        <v>387</v>
+      </c>
       <c r="E264" s="1" t="s">
         <v>29</v>
       </c>
@@ -6025,7 +6654,9 @@
       <c r="C265" s="2">
         <v>264</v>
       </c>
-      <c r="D265" s="1"/>
+      <c r="D265" s="1" t="s">
+        <v>386</v>
+      </c>
       <c r="E265" s="1" t="s">
         <v>28</v>
       </c>
@@ -6041,7 +6672,9 @@
       <c r="C266" s="2">
         <v>265</v>
       </c>
-      <c r="D266" s="1"/>
+      <c r="D266" s="1" t="s">
+        <v>387</v>
+      </c>
       <c r="E266" s="1" t="s">
         <v>29</v>
       </c>
@@ -6057,7 +6690,9 @@
       <c r="C267" s="2">
         <v>266</v>
       </c>
-      <c r="D267" s="1"/>
+      <c r="D267" s="1" t="s">
+        <v>386</v>
+      </c>
       <c r="E267" s="1" t="s">
         <v>28</v>
       </c>
@@ -6073,7 +6708,9 @@
       <c r="C268" s="2">
         <v>267</v>
       </c>
-      <c r="D268" s="1"/>
+      <c r="D268" s="1" t="s">
+        <v>457</v>
+      </c>
       <c r="E268" s="1" t="s">
         <v>275</v>
       </c>
@@ -6089,7 +6726,9 @@
       <c r="C269" s="2">
         <v>268</v>
       </c>
-      <c r="D269" s="1"/>
+      <c r="D269" s="1" t="s">
+        <v>458</v>
+      </c>
       <c r="E269" s="1" t="s">
         <v>276</v>
       </c>
@@ -6105,7 +6744,9 @@
       <c r="C270" s="2">
         <v>269</v>
       </c>
-      <c r="D270" s="1"/>
+      <c r="D270" s="1" t="s">
+        <v>459</v>
+      </c>
       <c r="E270" s="1" t="s">
         <v>277</v>
       </c>
@@ -6121,7 +6762,9 @@
       <c r="C271" s="2">
         <v>270</v>
       </c>
-      <c r="D271" s="1"/>
+      <c r="D271" s="1" t="s">
+        <v>460</v>
+      </c>
       <c r="E271" s="1" t="s">
         <v>278</v>
       </c>
@@ -6137,7 +6780,9 @@
       <c r="C272" s="2">
         <v>271</v>
       </c>
-      <c r="D272" s="1"/>
+      <c r="D272" s="1" t="s">
+        <v>457</v>
+      </c>
       <c r="E272" s="1" t="s">
         <v>275</v>
       </c>
@@ -6153,7 +6798,9 @@
       <c r="C273" s="2">
         <v>272</v>
       </c>
-      <c r="D273" s="1"/>
+      <c r="D273" s="1" t="s">
+        <v>458</v>
+      </c>
       <c r="E273" s="1" t="s">
         <v>276</v>
       </c>
@@ -6169,7 +6816,9 @@
       <c r="C274" s="2">
         <v>273</v>
       </c>
-      <c r="D274" s="1"/>
+      <c r="D274" s="1" t="s">
+        <v>459</v>
+      </c>
       <c r="E274" s="1" t="s">
         <v>277</v>
       </c>
@@ -6185,7 +6834,9 @@
       <c r="C275" s="2">
         <v>274</v>
       </c>
-      <c r="D275" s="1"/>
+      <c r="D275" s="1" t="s">
+        <v>460</v>
+      </c>
       <c r="E275" s="1" t="s">
         <v>278</v>
       </c>
@@ -6201,7 +6852,9 @@
       <c r="C276" s="2">
         <v>275</v>
       </c>
-      <c r="D276" s="1"/>
+      <c r="D276" s="1" t="s">
+        <v>457</v>
+      </c>
       <c r="E276" s="1" t="s">
         <v>281</v>
       </c>
@@ -6217,7 +6870,9 @@
       <c r="C277" s="2">
         <v>276</v>
       </c>
-      <c r="D277" s="1"/>
+      <c r="D277" s="1" t="s">
+        <v>458</v>
+      </c>
       <c r="E277" s="1" t="s">
         <v>282</v>
       </c>
@@ -6233,7 +6888,9 @@
       <c r="C278" s="2">
         <v>277</v>
       </c>
-      <c r="D278" s="1"/>
+      <c r="D278" s="1" t="s">
+        <v>459</v>
+      </c>
       <c r="E278" s="1" t="s">
         <v>277</v>
       </c>
@@ -6249,7 +6906,9 @@
       <c r="C279" s="2">
         <v>278</v>
       </c>
-      <c r="D279" s="1"/>
+      <c r="D279" s="1" t="s">
+        <v>460</v>
+      </c>
       <c r="E279" s="1" t="s">
         <v>278</v>
       </c>
@@ -6265,7 +6924,9 @@
       <c r="C280" s="2">
         <v>279</v>
       </c>
-      <c r="D280" s="1"/>
+      <c r="D280" s="1" t="s">
+        <v>461</v>
+      </c>
       <c r="E280" s="1" t="s">
         <v>284</v>
       </c>
@@ -6281,7 +6942,9 @@
       <c r="C281" s="2">
         <v>280</v>
       </c>
-      <c r="D281" s="1"/>
+      <c r="D281" s="1" t="s">
+        <v>462</v>
+      </c>
       <c r="E281" s="1" t="s">
         <v>285</v>
       </c>
@@ -6297,7 +6960,9 @@
       <c r="C282" s="2">
         <v>281</v>
       </c>
-      <c r="D282" s="1"/>
+      <c r="D282" s="1" t="s">
+        <v>463</v>
+      </c>
       <c r="E282" s="1" t="s">
         <v>286</v>
       </c>
@@ -6313,7 +6978,9 @@
       <c r="C283" s="2">
         <v>282</v>
       </c>
-      <c r="D283" s="1"/>
+      <c r="D283" s="1" t="s">
+        <v>464</v>
+      </c>
       <c r="E283" s="1" t="s">
         <v>287</v>
       </c>
@@ -6329,7 +6996,9 @@
       <c r="C284" s="2">
         <v>283</v>
       </c>
-      <c r="D284" s="1"/>
+      <c r="D284" s="1" t="s">
+        <v>465</v>
+      </c>
       <c r="E284" s="1" t="s">
         <v>288</v>
       </c>
@@ -6345,7 +7014,9 @@
       <c r="C285" s="2">
         <v>284</v>
       </c>
-      <c r="D285" s="1"/>
+      <c r="D285" s="1" t="s">
+        <v>466</v>
+      </c>
       <c r="E285" s="1" t="s">
         <v>289</v>
       </c>
@@ -6361,7 +7032,9 @@
       <c r="C286" s="2">
         <v>285</v>
       </c>
-      <c r="D286" s="1"/>
+      <c r="D286" s="1" t="s">
+        <v>291</v>
+      </c>
       <c r="E286" s="1" t="s">
         <v>290</v>
       </c>
@@ -6391,7 +7064,9 @@
       <c r="C288" s="2">
         <v>287</v>
       </c>
-      <c r="D288" s="1"/>
+      <c r="D288" s="1" t="s">
+        <v>467</v>
+      </c>
       <c r="E288" s="1" t="s">
         <v>293</v>
       </c>
@@ -6407,7 +7082,9 @@
       <c r="C289" s="2">
         <v>288</v>
       </c>
-      <c r="D289" s="1"/>
+      <c r="D289" s="1" t="s">
+        <v>468</v>
+      </c>
       <c r="E289" s="1" t="s">
         <v>294</v>
       </c>
@@ -6423,7 +7100,9 @@
       <c r="C290" s="2">
         <v>289</v>
       </c>
-      <c r="D290" s="1"/>
+      <c r="D290" s="1" t="s">
+        <v>469</v>
+      </c>
       <c r="E290" s="1" t="s">
         <v>295</v>
       </c>
@@ -6439,7 +7118,9 @@
       <c r="C291" s="2">
         <v>290</v>
       </c>
-      <c r="D291" s="1"/>
+      <c r="D291" s="1" t="s">
+        <v>470</v>
+      </c>
       <c r="E291" s="1" t="s">
         <v>296</v>
       </c>
@@ -6455,7 +7136,9 @@
       <c r="C292" s="2">
         <v>291</v>
       </c>
-      <c r="D292" s="1"/>
+      <c r="D292" s="1" t="s">
+        <v>291</v>
+      </c>
       <c r="E292" s="1" t="s">
         <v>290</v>
       </c>
@@ -6485,7 +7168,9 @@
       <c r="C294" s="2">
         <v>293</v>
       </c>
-      <c r="D294" s="1"/>
+      <c r="D294" s="1" t="s">
+        <v>471</v>
+      </c>
       <c r="E294" s="1" t="s">
         <v>298</v>
       </c>
@@ -6501,7 +7186,9 @@
       <c r="C295" s="2">
         <v>294</v>
       </c>
-      <c r="D295" s="1"/>
+      <c r="D295" s="1" t="s">
+        <v>464</v>
+      </c>
       <c r="E295" s="1" t="s">
         <v>287</v>
       </c>
@@ -6517,7 +7204,9 @@
       <c r="C296" s="2">
         <v>295</v>
       </c>
-      <c r="D296" s="1"/>
+      <c r="D296" s="1" t="s">
+        <v>472</v>
+      </c>
       <c r="E296" s="1" t="s">
         <v>299</v>
       </c>
@@ -6533,7 +7222,9 @@
       <c r="C297" s="2">
         <v>296</v>
       </c>
-      <c r="D297" s="1"/>
+      <c r="D297" s="1" t="s">
+        <v>473</v>
+      </c>
       <c r="E297" s="1" t="s">
         <v>300</v>
       </c>
@@ -6549,7 +7240,9 @@
       <c r="C298" s="2">
         <v>297</v>
       </c>
-      <c r="D298" s="1"/>
+      <c r="D298" s="1" t="s">
+        <v>474</v>
+      </c>
       <c r="E298" s="1" t="s">
         <v>301</v>
       </c>
@@ -6565,7 +7258,9 @@
       <c r="C299" s="2">
         <v>298</v>
       </c>
-      <c r="D299" s="1"/>
+      <c r="D299" s="1" t="s">
+        <v>475</v>
+      </c>
       <c r="E299" s="1" t="s">
         <v>302</v>
       </c>
@@ -6581,7 +7276,9 @@
       <c r="C300" s="2">
         <v>299</v>
       </c>
-      <c r="D300" s="1"/>
+      <c r="D300" s="1" t="s">
+        <v>476</v>
+      </c>
       <c r="E300" s="1" t="s">
         <v>303</v>
       </c>
@@ -6597,7 +7294,9 @@
       <c r="C301" s="2">
         <v>300</v>
       </c>
-      <c r="D301" s="1"/>
+      <c r="D301" s="1" t="s">
+        <v>477</v>
+      </c>
       <c r="E301" s="1" t="s">
         <v>304</v>
       </c>
@@ -6613,7 +7312,9 @@
       <c r="C302" s="2">
         <v>301</v>
       </c>
-      <c r="D302" s="1"/>
+      <c r="D302" s="1" t="s">
+        <v>478</v>
+      </c>
       <c r="E302" s="1" t="s">
         <v>305</v>
       </c>
@@ -6629,7 +7330,9 @@
       <c r="C303" s="2">
         <v>302</v>
       </c>
-      <c r="D303" s="1"/>
+      <c r="D303" s="1" t="s">
+        <v>479</v>
+      </c>
       <c r="E303" s="1" t="s">
         <v>306</v>
       </c>
@@ -6645,7 +7348,9 @@
       <c r="C304" s="2">
         <v>303</v>
       </c>
-      <c r="D304" s="1"/>
+      <c r="D304" s="1" t="s">
+        <v>480</v>
+      </c>
       <c r="E304" s="1" t="s">
         <v>307</v>
       </c>
@@ -6661,7 +7366,9 @@
       <c r="C305" s="2">
         <v>304</v>
       </c>
-      <c r="D305" s="1"/>
+      <c r="D305" s="1" t="s">
+        <v>481</v>
+      </c>
       <c r="E305" s="1" t="s">
         <v>308</v>
       </c>
@@ -6677,7 +7384,9 @@
       <c r="C306" s="2">
         <v>305</v>
       </c>
-      <c r="D306" s="1"/>
+      <c r="D306" s="1" t="s">
+        <v>471</v>
+      </c>
       <c r="E306" s="1" t="s">
         <v>298</v>
       </c>
@@ -6693,7 +7402,9 @@
       <c r="C307" s="2">
         <v>306</v>
       </c>
-      <c r="D307" s="1"/>
+      <c r="D307" s="1" t="s">
+        <v>464</v>
+      </c>
       <c r="E307" s="1" t="s">
         <v>287</v>
       </c>
@@ -6709,7 +7420,9 @@
       <c r="C308" s="2">
         <v>307</v>
       </c>
-      <c r="D308" s="1"/>
+      <c r="D308" s="1" t="s">
+        <v>472</v>
+      </c>
       <c r="E308" s="1" t="s">
         <v>299</v>
       </c>
@@ -6725,7 +7438,9 @@
       <c r="C309" s="2">
         <v>308</v>
       </c>
-      <c r="D309" s="1"/>
+      <c r="D309" s="1" t="s">
+        <v>473</v>
+      </c>
       <c r="E309" s="1" t="s">
         <v>300</v>
       </c>
@@ -6741,7 +7456,9 @@
       <c r="C310" s="2">
         <v>309</v>
       </c>
-      <c r="D310" s="1"/>
+      <c r="D310" s="1" t="s">
+        <v>474</v>
+      </c>
       <c r="E310" s="1" t="s">
         <v>301</v>
       </c>
@@ -6757,7 +7474,9 @@
       <c r="C311" s="2">
         <v>310</v>
       </c>
-      <c r="D311" s="1"/>
+      <c r="D311" s="1" t="s">
+        <v>475</v>
+      </c>
       <c r="E311" s="1" t="s">
         <v>302</v>
       </c>
@@ -6773,7 +7492,9 @@
       <c r="C312" s="2">
         <v>311</v>
       </c>
-      <c r="D312" s="1"/>
+      <c r="D312" s="1" t="s">
+        <v>476</v>
+      </c>
       <c r="E312" s="1" t="s">
         <v>303</v>
       </c>
@@ -6789,7 +7510,9 @@
       <c r="C313" s="2">
         <v>312</v>
       </c>
-      <c r="D313" s="1"/>
+      <c r="D313" s="1" t="s">
+        <v>477</v>
+      </c>
       <c r="E313" s="1" t="s">
         <v>304</v>
       </c>
@@ -6805,7 +7528,9 @@
       <c r="C314" s="2">
         <v>313</v>
       </c>
-      <c r="D314" s="1"/>
+      <c r="D314" s="1" t="s">
+        <v>478</v>
+      </c>
       <c r="E314" s="1" t="s">
         <v>305</v>
       </c>
@@ -6821,7 +7546,9 @@
       <c r="C315" s="2">
         <v>314</v>
       </c>
-      <c r="D315" s="1"/>
+      <c r="D315" s="1" t="s">
+        <v>479</v>
+      </c>
       <c r="E315" s="1" t="s">
         <v>306</v>
       </c>
@@ -6837,7 +7564,9 @@
       <c r="C316" s="2">
         <v>315</v>
       </c>
-      <c r="D316" s="1"/>
+      <c r="D316" s="1" t="s">
+        <v>480</v>
+      </c>
       <c r="E316" s="1" t="s">
         <v>307</v>
       </c>
@@ -6853,7 +7582,9 @@
       <c r="C317" s="2">
         <v>316</v>
       </c>
-      <c r="D317" s="1"/>
+      <c r="D317" s="1" t="s">
+        <v>481</v>
+      </c>
       <c r="E317" s="1" t="s">
         <v>308</v>
       </c>
@@ -6869,7 +7600,9 @@
       <c r="C318" s="2">
         <v>317</v>
       </c>
-      <c r="D318" s="1"/>
+      <c r="D318" s="1" t="s">
+        <v>512</v>
+      </c>
       <c r="E318" s="1" t="s">
         <v>311</v>
       </c>
@@ -6885,7 +7618,9 @@
       <c r="C319" s="2">
         <v>318</v>
       </c>
-      <c r="D319" s="1"/>
+      <c r="D319" s="1" t="s">
+        <v>513</v>
+      </c>
       <c r="E319" s="1" t="s">
         <v>312</v>
       </c>
@@ -6901,7 +7636,9 @@
       <c r="C320" s="2">
         <v>319</v>
       </c>
-      <c r="D320" s="1"/>
+      <c r="D320" s="1" t="s">
+        <v>514</v>
+      </c>
       <c r="E320" s="1" t="s">
         <v>313</v>
       </c>
@@ -7375,7 +8112,9 @@
       <c r="C350" s="2">
         <v>349</v>
       </c>
-      <c r="D350" s="1"/>
+      <c r="D350" s="1" t="s">
+        <v>507</v>
+      </c>
       <c r="E350" s="1" t="s">
         <v>340</v>
       </c>
@@ -7391,7 +8130,9 @@
       <c r="C351" s="2">
         <v>350</v>
       </c>
-      <c r="D351" s="1"/>
+      <c r="D351" s="1" t="s">
+        <v>508</v>
+      </c>
       <c r="E351" s="1" t="s">
         <v>341</v>
       </c>
@@ -7407,7 +8148,9 @@
       <c r="C352" s="2">
         <v>351</v>
       </c>
-      <c r="D352" s="1"/>
+      <c r="D352" s="1" t="s">
+        <v>511</v>
+      </c>
       <c r="E352" s="1" t="s">
         <v>342</v>
       </c>
@@ -7423,7 +8166,9 @@
       <c r="C353" s="2">
         <v>352</v>
       </c>
-      <c r="D353" s="1"/>
+      <c r="D353" s="1" t="s">
+        <v>509</v>
+      </c>
       <c r="E353" s="1" t="s">
         <v>343</v>
       </c>
@@ -7439,7 +8184,9 @@
       <c r="C354" s="2">
         <v>353</v>
       </c>
-      <c r="D354" s="1"/>
+      <c r="D354" s="1" t="s">
+        <v>406</v>
+      </c>
       <c r="E354" s="1" t="s">
         <v>344</v>
       </c>
@@ -7455,7 +8202,9 @@
       <c r="C355" s="2">
         <v>354</v>
       </c>
-      <c r="D355" s="1"/>
+      <c r="D355" s="1" t="s">
+        <v>510</v>
+      </c>
       <c r="E355" s="1" t="s">
         <v>345</v>
       </c>
@@ -7471,7 +8220,9 @@
       <c r="C356" s="2">
         <v>355</v>
       </c>
-      <c r="D356" s="1"/>
+      <c r="D356" s="1" t="s">
+        <v>291</v>
+      </c>
       <c r="E356" s="1" t="s">
         <v>346</v>
       </c>
@@ -7487,7 +8238,9 @@
       <c r="C357" s="2">
         <v>356</v>
       </c>
-      <c r="D357" s="1"/>
+      <c r="D357" s="1" t="s">
+        <v>407</v>
+      </c>
       <c r="E357" s="1" t="s">
         <v>347</v>
       </c>
@@ -7517,7 +8270,9 @@
       <c r="C359" s="2">
         <v>358</v>
       </c>
-      <c r="D359" s="1"/>
+      <c r="D359" s="1" t="s">
+        <v>500</v>
+      </c>
       <c r="E359" s="1" t="s">
         <v>349</v>
       </c>
@@ -7533,7 +8288,9 @@
       <c r="C360" s="2">
         <v>359</v>
       </c>
-      <c r="D360" s="1"/>
+      <c r="D360" s="1" t="s">
+        <v>501</v>
+      </c>
       <c r="E360" s="1" t="s">
         <v>350</v>
       </c>
@@ -7549,7 +8306,9 @@
       <c r="C361" s="2">
         <v>360</v>
       </c>
-      <c r="D361" s="1"/>
+      <c r="D361" s="1" t="s">
+        <v>502</v>
+      </c>
       <c r="E361" s="1" t="s">
         <v>351</v>
       </c>
@@ -7565,7 +8324,9 @@
       <c r="C362" s="2">
         <v>361</v>
       </c>
-      <c r="D362" s="1"/>
+      <c r="D362" s="1" t="s">
+        <v>503</v>
+      </c>
       <c r="E362" s="1" t="s">
         <v>352</v>
       </c>
@@ -7581,7 +8342,9 @@
       <c r="C363" s="2">
         <v>362</v>
       </c>
-      <c r="D363" s="4"/>
+      <c r="D363" s="1" t="s">
+        <v>504</v>
+      </c>
       <c r="E363" s="4" t="s">
         <v>353</v>
       </c>
@@ -7597,7 +8360,9 @@
       <c r="C364" s="2">
         <v>363</v>
       </c>
-      <c r="D364" s="4"/>
+      <c r="D364" s="1" t="s">
+        <v>505</v>
+      </c>
       <c r="E364" s="4" t="s">
         <v>354</v>
       </c>
@@ -7613,7 +8378,9 @@
       <c r="C365" s="2">
         <v>364</v>
       </c>
-      <c r="D365" s="4"/>
+      <c r="D365" s="1" t="s">
+        <v>506</v>
+      </c>
       <c r="E365" s="4" t="s">
         <v>355</v>
       </c>
@@ -7629,7 +8396,9 @@
       <c r="C366" s="2">
         <v>365</v>
       </c>
-      <c r="D366" s="4"/>
+      <c r="D366" s="1" t="s">
+        <v>291</v>
+      </c>
       <c r="E366" s="4" t="s">
         <v>346</v>
       </c>
@@ -7645,7 +8414,9 @@
       <c r="C367" s="2">
         <v>366</v>
       </c>
-      <c r="D367" s="4"/>
+      <c r="D367" s="1" t="s">
+        <v>407</v>
+      </c>
       <c r="E367" s="4" t="s">
         <v>347</v>
       </c>
@@ -7675,7 +8446,9 @@
       <c r="C369" s="2">
         <v>368</v>
       </c>
-      <c r="D369" s="4"/>
+      <c r="D369" s="1" t="s">
+        <v>482</v>
+      </c>
       <c r="E369" s="4" t="s">
         <v>357</v>
       </c>
@@ -7691,7 +8464,9 @@
       <c r="C370" s="2">
         <v>369</v>
       </c>
-      <c r="D370" s="4"/>
+      <c r="D370" s="1" t="s">
+        <v>483</v>
+      </c>
       <c r="E370" s="4" t="s">
         <v>358</v>
       </c>
@@ -7707,7 +8482,9 @@
       <c r="C371" s="2">
         <v>370</v>
       </c>
-      <c r="D371" s="4"/>
+      <c r="D371" s="1" t="s">
+        <v>484</v>
+      </c>
       <c r="E371" s="4" t="s">
         <v>359</v>
       </c>
@@ -7723,7 +8500,9 @@
       <c r="C372" s="2">
         <v>371</v>
       </c>
-      <c r="D372" s="4"/>
+      <c r="D372" s="1" t="s">
+        <v>291</v>
+      </c>
       <c r="E372" s="4" t="s">
         <v>290</v>
       </c>
@@ -7753,7 +8532,9 @@
       <c r="C374" s="2">
         <v>373</v>
       </c>
-      <c r="D374" s="4"/>
+      <c r="D374" s="1" t="s">
+        <v>361</v>
+      </c>
       <c r="E374" s="4" t="s">
         <v>361</v>
       </c>
@@ -7769,7 +8550,9 @@
       <c r="C375" s="2">
         <v>374</v>
       </c>
-      <c r="D375" s="4"/>
+      <c r="D375" s="1" t="s">
+        <v>362</v>
+      </c>
       <c r="E375" s="4" t="s">
         <v>362</v>
       </c>
@@ -7785,7 +8568,9 @@
       <c r="C376" s="2">
         <v>375</v>
       </c>
-      <c r="D376" s="4"/>
+      <c r="D376" s="1" t="s">
+        <v>363</v>
+      </c>
       <c r="E376" s="4" t="s">
         <v>363</v>
       </c>
@@ -7801,7 +8586,9 @@
       <c r="C377" s="2">
         <v>376</v>
       </c>
-      <c r="D377" s="4"/>
+      <c r="D377" s="1" t="s">
+        <v>364</v>
+      </c>
       <c r="E377" s="4" t="s">
         <v>364</v>
       </c>
@@ -7817,7 +8604,9 @@
       <c r="C378" s="2">
         <v>377</v>
       </c>
-      <c r="D378" s="4"/>
+      <c r="D378" s="1" t="s">
+        <v>365</v>
+      </c>
       <c r="E378" s="4" t="s">
         <v>365</v>
       </c>
@@ -7833,7 +8622,9 @@
       <c r="C379" s="2">
         <v>378</v>
       </c>
-      <c r="D379" s="4"/>
+      <c r="D379" s="1" t="s">
+        <v>366</v>
+      </c>
       <c r="E379" s="4" t="s">
         <v>366</v>
       </c>
@@ -7849,7 +8640,9 @@
       <c r="C380" s="2">
         <v>379</v>
       </c>
-      <c r="D380" s="4"/>
+      <c r="D380" s="1" t="s">
+        <v>367</v>
+      </c>
       <c r="E380" s="4" t="s">
         <v>367</v>
       </c>
@@ -7865,7 +8658,9 @@
       <c r="C381" s="2">
         <v>380</v>
       </c>
-      <c r="D381" s="4"/>
+      <c r="D381" s="1" t="s">
+        <v>290</v>
+      </c>
       <c r="E381" s="4" t="s">
         <v>290</v>
       </c>
@@ -9281,7 +10076,9 @@
       <c r="C460" s="2">
         <v>459</v>
       </c>
-      <c r="D460" s="4"/>
+      <c r="D460" s="1" t="s">
+        <v>485</v>
+      </c>
       <c r="E460" s="4" t="s">
         <v>370</v>
       </c>
@@ -9297,7 +10094,9 @@
       <c r="C461" s="2">
         <v>460</v>
       </c>
-      <c r="D461" s="4"/>
+      <c r="D461" s="1" t="s">
+        <v>486</v>
+      </c>
       <c r="E461" s="4" t="s">
         <v>371</v>
       </c>
@@ -9313,7 +10112,9 @@
       <c r="C462" s="2">
         <v>461</v>
       </c>
-      <c r="D462" s="4"/>
+      <c r="D462" s="1" t="s">
+        <v>487</v>
+      </c>
       <c r="E462" s="4" t="s">
         <v>372</v>
       </c>
@@ -9329,7 +10130,9 @@
       <c r="C463" s="2">
         <v>462</v>
       </c>
-      <c r="D463" s="4"/>
+      <c r="D463" s="1" t="s">
+        <v>488</v>
+      </c>
       <c r="E463" s="4" t="s">
         <v>373</v>
       </c>
@@ -9345,7 +10148,9 @@
       <c r="C464" s="2">
         <v>463</v>
       </c>
-      <c r="D464" s="4"/>
+      <c r="D464" s="1" t="s">
+        <v>489</v>
+      </c>
       <c r="E464" s="4" t="s">
         <v>374</v>
       </c>
@@ -9361,7 +10166,9 @@
       <c r="C465" s="2">
         <v>464</v>
       </c>
-      <c r="D465" s="4"/>
+      <c r="D465" s="1" t="s">
+        <v>490</v>
+      </c>
       <c r="E465" s="4" t="s">
         <v>375</v>
       </c>
@@ -9377,7 +10184,9 @@
       <c r="C466" s="2">
         <v>465</v>
       </c>
-      <c r="D466" s="4"/>
+      <c r="D466" s="1" t="s">
+        <v>491</v>
+      </c>
       <c r="E466" s="4" t="s">
         <v>376</v>
       </c>
@@ -9393,7 +10202,9 @@
       <c r="C467" s="2">
         <v>466</v>
       </c>
-      <c r="D467" s="4"/>
+      <c r="D467" s="1" t="s">
+        <v>492</v>
+      </c>
       <c r="E467" s="4" t="s">
         <v>377</v>
       </c>
@@ -9409,7 +10220,9 @@
       <c r="C468" s="2">
         <v>467</v>
       </c>
-      <c r="D468" s="4"/>
+      <c r="D468" s="1" t="s">
+        <v>493</v>
+      </c>
       <c r="E468" s="4" t="s">
         <v>378</v>
       </c>
@@ -9425,7 +10238,9 @@
       <c r="C469" s="2">
         <v>468</v>
       </c>
-      <c r="D469" s="4"/>
+      <c r="D469" s="1" t="s">
+        <v>494</v>
+      </c>
       <c r="E469" s="4" t="s">
         <v>379</v>
       </c>
@@ -9441,7 +10256,9 @@
       <c r="C470" s="2">
         <v>469</v>
       </c>
-      <c r="D470" s="4"/>
+      <c r="D470" s="1" t="s">
+        <v>495</v>
+      </c>
       <c r="E470" s="4" t="s">
         <v>380</v>
       </c>
@@ -9457,7 +10274,9 @@
       <c r="C471" s="2">
         <v>470</v>
       </c>
-      <c r="D471" s="4"/>
+      <c r="D471" s="1" t="s">
+        <v>496</v>
+      </c>
       <c r="E471" s="4" t="s">
         <v>381</v>
       </c>
@@ -9473,7 +10292,9 @@
       <c r="C472" s="2">
         <v>471</v>
       </c>
-      <c r="D472" s="4"/>
+      <c r="D472" s="1" t="s">
+        <v>497</v>
+      </c>
       <c r="E472" s="4" t="s">
         <v>382</v>
       </c>
@@ -9489,7 +10310,9 @@
       <c r="C473" s="2">
         <v>472</v>
       </c>
-      <c r="D473" s="4"/>
+      <c r="D473" s="1" t="s">
+        <v>498</v>
+      </c>
       <c r="E473" s="4" t="s">
         <v>383</v>
       </c>
@@ -9505,7 +10328,9 @@
       <c r="C474" s="2">
         <v>473</v>
       </c>
-      <c r="D474" s="4"/>
+      <c r="D474" s="1" t="s">
+        <v>499</v>
+      </c>
       <c r="E474" s="4" t="s">
         <v>384</v>
       </c>
@@ -9521,7 +10346,9 @@
       <c r="C475" s="2">
         <v>474</v>
       </c>
-      <c r="D475" s="4"/>
+      <c r="D475" s="1" t="s">
+        <v>291</v>
+      </c>
       <c r="E475" s="4" t="s">
         <v>290</v>
       </c>
@@ -9540,6 +10367,159 @@
       <c r="D476" s="4"/>
       <c r="E476" s="4"/>
       <c r="F476" s="4"/>
+    </row>
+    <row r="477" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A477" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="B477" s="2">
+        <v>1</v>
+      </c>
+      <c r="C477" s="2">
+        <v>476</v>
+      </c>
+      <c r="D477" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="E477" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="478" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A478" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="B478" s="2">
+        <v>2</v>
+      </c>
+      <c r="C478" s="2">
+        <v>477</v>
+      </c>
+      <c r="D478" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="E478" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="479" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A479" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="B479" s="2">
+        <v>3</v>
+      </c>
+      <c r="C479" s="2">
+        <v>478</v>
+      </c>
+      <c r="D479" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="E479" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="480" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A480" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="B480" s="2">
+        <v>4</v>
+      </c>
+      <c r="C480" s="2">
+        <v>479</v>
+      </c>
+      <c r="D480" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="E480" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="481" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A481" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="B481" s="2">
+        <v>5</v>
+      </c>
+      <c r="C481" s="2">
+        <v>480</v>
+      </c>
+      <c r="D481" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="E481" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="482" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A482" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="B482" s="2">
+        <v>6</v>
+      </c>
+      <c r="C482" s="2">
+        <v>481</v>
+      </c>
+      <c r="D482" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="E482" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="483" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A483" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="B483" s="2">
+        <v>7</v>
+      </c>
+      <c r="C483" s="2">
+        <v>482</v>
+      </c>
+      <c r="D483" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="E483" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="484" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A484" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="B484" s="2">
+        <v>8</v>
+      </c>
+      <c r="C484" s="2">
+        <v>483</v>
+      </c>
+      <c r="D484" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="E484" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="485" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A485" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="B485" s="2">
+        <v>9</v>
+      </c>
+      <c r="C485" s="2">
+        <v>484</v>
+      </c>
+      <c r="D485" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="E485" s="1" t="s">
+        <v>325</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>